<commit_message>
Metni Sütünlara dönüştürme ve Formül ile ve & işareti ile birleştirme
</commit_message>
<xml_diff>
--- a/working 11.xlsx
+++ b/working 11.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
     <sheet name="Sayfa2" sheetId="2" r:id="rId2"/>
     <sheet name="Sayfa3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sayfa4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>FORMULLERİ BAŞKA HÜCRELERE TAŞIMA VE KOPYALAMA</t>
   </si>
@@ -96,6 +97,42 @@
   </si>
   <si>
     <t xml:space="preserve">Fatma </t>
+  </si>
+  <si>
+    <t>Fatma TEKBAŞ</t>
+  </si>
+  <si>
+    <t>Damla TEKİNERDOĞEN</t>
+  </si>
+  <si>
+    <t>Miraç SIKTAŞ</t>
+  </si>
+  <si>
+    <t>Kübra KALKANCI</t>
+  </si>
+  <si>
+    <t>Nurettin İĞDE</t>
+  </si>
+  <si>
+    <t>Mehmet ÇEVİKOL</t>
+  </si>
+  <si>
+    <t>Fatma BEN TEKBAŞ</t>
+  </si>
+  <si>
+    <t>Damla BEN TEKİNERDOĞEN</t>
+  </si>
+  <si>
+    <t>Miraç BEN SIKTAŞ</t>
+  </si>
+  <si>
+    <t>Kübra BEN KALKANCI</t>
+  </si>
+  <si>
+    <t>Nurettin BEN İĞDE</t>
+  </si>
+  <si>
+    <t>Mehmet BEN ÇEVİKOL</t>
   </si>
 </sst>
 </file>
@@ -142,7 +179,7 @@
       <name val="Arial Tur"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +228,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -394,21 +437,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -442,14 +551,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -464,6 +566,59 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,6 +639,77 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Yuvarlatılmış Dikdörtgen 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10462260" y="632460"/>
+          <a:ext cx="2545080" cy="1623060"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>EXCEL'DE BİRLEŞTİR FONKSİYONU VE İŞARETİ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -758,119 +984,119 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="5">
         <f ca="1">RANDBETWEEN(30,100)</f>
-        <v>62</v>
-      </c>
-      <c r="B4" s="9">
-        <f t="shared" ref="B4:D8" ca="1" si="0">RANDBETWEEN(30,100)</f>
-        <v>41</v>
-      </c>
-      <c r="C4" s="9">
+        <v>100</v>
+      </c>
+      <c r="B4" s="6">
+        <f t="shared" ref="B4:C8" ca="1" si="0">RANDBETWEEN(30,100)</f>
+        <v>64</v>
+      </c>
+      <c r="C4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="D4" s="10">
+        <v>82</v>
+      </c>
+      <c r="D4" s="7">
         <f ca="1">SUM(A4:C4)</f>
-        <v>162</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <f t="shared" ref="A5:A8" ca="1" si="1">RANDBETWEEN(30,100)</f>
-        <v>73</v>
-      </c>
-      <c r="B5" s="5">
+        <v>94</v>
+      </c>
+      <c r="B5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="C5" s="5">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" ref="D5:D8" ca="1" si="2">SUM(A5:C5)</f>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B7" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>68</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" ref="D5:D8" ca="1" si="2">SUM(A5:C5)</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="C7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" ca="1" si="2"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="B6" s="5">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="C6" s="5">
+        <v>82</v>
+      </c>
+      <c r="C8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="D6" s="10">
+        <v>39</v>
+      </c>
+      <c r="D8" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="B7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="C7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="D7" s="10">
-        <f t="shared" ca="1" si="2"/>
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="B8" s="7">
-        <f t="shared" ca="1" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="C8" s="7">
-        <f t="shared" ca="1" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="D8" s="14">
-        <f t="shared" ca="1" si="2"/>
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -893,25 +1119,25 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
       <c r="G3">
         <v>8</v>
       </c>
@@ -921,31 +1147,31 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
       <c r="G4">
         <v>6</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="12">
         <f>G3*(G4+G5)/G6</f>
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
       <c r="G5">
         <v>4</v>
       </c>
@@ -955,14 +1181,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
       <c r="G6">
         <v>2</v>
       </c>
@@ -972,23 +1198,23 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -999,8 +1225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,226 +1235,226 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="3" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="19">
         <v>589</v>
       </c>
-      <c r="H3" s="25">
+      <c r="H3" s="19">
         <v>632</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="20">
         <v>58</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="20">
         <v>96</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="20">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="19">
         <v>589</v>
       </c>
-      <c r="H4" s="25">
+      <c r="H4" s="19">
         <v>634</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="20">
         <v>58</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="20">
         <v>96</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="20">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="19">
         <v>589</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="19">
         <v>636</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="20">
         <v>58</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="20">
         <v>96</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="20">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="19">
         <v>589</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="19">
         <v>638</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="20">
         <v>58</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="20">
         <v>96</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="20">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="19">
         <v>589</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="19">
         <v>640</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="20">
         <v>58</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="20">
         <v>96</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="20">
         <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="19">
         <v>589</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="19">
         <v>642</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="20">
         <v>58</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="20">
         <v>96</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="20">
         <v>42</v>
       </c>
     </row>
@@ -1275,4 +1501,395 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="e">
+        <f>CONCATENATE(#REF!," ",#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B1" s="35" t="str">
+        <f>CONCATENATE(C1,",",D1)</f>
+        <v>Fatma ,TEKBAŞ</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="35" t="str">
+        <f>CONCATENATE(F1,"-",G1)</f>
+        <v>Fatma-TEKBAŞ</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="38">
+        <v>589</v>
+      </c>
+      <c r="I1" s="38">
+        <v>632</v>
+      </c>
+      <c r="J1" s="39">
+        <v>58</v>
+      </c>
+      <c r="K1" s="39">
+        <v>96</v>
+      </c>
+      <c r="L1" s="40">
+        <v>32</v>
+      </c>
+      <c r="M1" t="str">
+        <f>F1&amp;" BEN "&amp;G1</f>
+        <v>Fatma BEN TEKBAŞ</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="e">
+        <f>CONCATENATE(#REF!," ",#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B2" s="27" t="str">
+        <f t="shared" ref="B2:B6" si="0">CONCATENATE(C2,",",D2)</f>
+        <v>Damla,TEKİNERDOĞEN</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="35" t="str">
+        <f t="shared" ref="E2:E6" si="1">CONCATENATE(F2,"-",G2)</f>
+        <v>Damla-TEKİNERDOĞEN</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="30">
+        <v>589</v>
+      </c>
+      <c r="I2" s="30">
+        <v>634</v>
+      </c>
+      <c r="J2" s="31">
+        <v>58</v>
+      </c>
+      <c r="K2" s="31">
+        <v>96</v>
+      </c>
+      <c r="L2" s="42">
+        <v>34</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M6" si="2">F2&amp;" BEN "&amp;G2</f>
+        <v>Damla BEN TEKİNERDOĞEN</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="41" t="e">
+        <f>CONCATENATE(#REF!," ",#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B3" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>Miraç,SIKTAŞ</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>Miraç-SIKTAŞ</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="30">
+        <v>589</v>
+      </c>
+      <c r="I3" s="30">
+        <v>636</v>
+      </c>
+      <c r="J3" s="31">
+        <v>58</v>
+      </c>
+      <c r="K3" s="31">
+        <v>96</v>
+      </c>
+      <c r="L3" s="42">
+        <v>36</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="2"/>
+        <v>Miraç BEN SIKTAŞ</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="41" t="e">
+        <f>CONCATENATE(#REF!," ",#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B4" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>Kübra,KALKANCI</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>Kübra-KALKANCI</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="30">
+        <v>589</v>
+      </c>
+      <c r="I4" s="30">
+        <v>638</v>
+      </c>
+      <c r="J4" s="31">
+        <v>58</v>
+      </c>
+      <c r="K4" s="31">
+        <v>96</v>
+      </c>
+      <c r="L4" s="42">
+        <v>38</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="2"/>
+        <v>Kübra BEN KALKANCI</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="41" t="e">
+        <f>CONCATENATE(#REF!," ",#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B5" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>Nurettin,İĞDE</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>Nurettin-İĞDE</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="30">
+        <v>589</v>
+      </c>
+      <c r="I5" s="30">
+        <v>640</v>
+      </c>
+      <c r="J5" s="31">
+        <v>58</v>
+      </c>
+      <c r="K5" s="31">
+        <v>96</v>
+      </c>
+      <c r="L5" s="42">
+        <v>40</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="2"/>
+        <v>Nurettin BEN İĞDE</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="e">
+        <f>CONCATENATE(#REF!," ",#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B6" s="44" t="str">
+        <f t="shared" si="0"/>
+        <v>Mehmet,ÇEVİKOL</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>Mehmet-ÇEVİKOL</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="47">
+        <v>589</v>
+      </c>
+      <c r="I6" s="47">
+        <v>642</v>
+      </c>
+      <c r="J6" s="48">
+        <v>58</v>
+      </c>
+      <c r="K6" s="48">
+        <v>96</v>
+      </c>
+      <c r="L6" s="49">
+        <v>42</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="2"/>
+        <v>Mehmet BEN ÇEVİKOL</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="str">
+        <f>CONCATENATE(H1,I1)</f>
+        <v>589632</v>
+      </c>
+      <c r="J8" t="str">
+        <f>CONCATENATE(J1," - ",K1," - ",L1)</f>
+        <v>58 - 96 - 32</v>
+      </c>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" ref="H9:H13" si="3">CONCATENATE(H2,I2)</f>
+        <v>589634</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ref="J9:J13" si="4">CONCATENATE(J2," - ",K2," - ",L2)</f>
+        <v>58 - 96 - 34</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>589636</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="4"/>
+        <v>58 - 96 - 36</v>
+      </c>
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>589638</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="4"/>
+        <v>58 - 96 - 38</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>589640</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="4"/>
+        <v>58 - 96 - 40</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>589642</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="4"/>
+        <v>58 - 96 - 42</v>
+      </c>
+      <c r="M13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>